<commit_message>
updates to working filenotebook
</commit_message>
<xml_diff>
--- a/CensusBuildingPermits2000_2018.xlsx
+++ b/CensusBuildingPermits2000_2018.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/staceyterrell/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/staceyterrell/Project-Orange/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE6F8D4-3843-9647-9B92-CE54462D0647}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{649EE218-BC4D-0445-8EE4-9BA82C3ABFCB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1780" yWindow="460" windowWidth="28040" windowHeight="16500" xr2:uid="{4C203B42-FFBF-3643-8253-9F198F792B04}"/>
+    <workbookView xWindow="760" yWindow="460" windowWidth="28040" windowHeight="16500" xr2:uid="{4C203B42-FFBF-3643-8253-9F198F792B04}"/>
   </bookViews>
   <sheets>
-    <sheet name="Building Permits Census" sheetId="1" r:id="rId1"/>
+    <sheet name="CensusBuildingPermits2000_2018" sheetId="2" r:id="rId1"/>
+    <sheet name="Building Permits Census" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="22">
   <si>
     <t>288 26420 Houston-The Woodlands-Sugar Land,</t>
   </si>
@@ -107,12 +108,19 @@
   <si>
     <t>Austin County – 28,417</t>
   </si>
+  <si>
+    <t>Year</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -159,6 +167,26 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -177,19 +205,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -218,8 +255,8 @@
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>317500</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -569,11 +606,250 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DEAF8D7-952D-CB4C-A41E-816768BE26B6}">
+  <dimension ref="A1:C20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="11.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" style="7" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="7">
+        <v>2018</v>
+      </c>
+      <c r="B2" s="8">
+        <v>57288</v>
+      </c>
+      <c r="C2" s="8">
+        <v>9172451</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="7">
+        <v>2017</v>
+      </c>
+      <c r="B3" s="8">
+        <v>42395</v>
+      </c>
+      <c r="C3" s="10">
+        <v>7880444</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="7">
+        <v>2016</v>
+      </c>
+      <c r="B4" s="8">
+        <v>44732</v>
+      </c>
+      <c r="C4" s="8">
+        <v>7395665</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>2015</v>
+      </c>
+      <c r="B5" s="9">
+        <v>56901</v>
+      </c>
+      <c r="C5" s="10">
+        <v>8566382</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <v>2014</v>
+      </c>
+      <c r="B6" s="9">
+        <v>63749</v>
+      </c>
+      <c r="C6" s="10">
+        <v>9252773</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>2013</v>
+      </c>
+      <c r="B7" s="9">
+        <v>51333</v>
+      </c>
+      <c r="C7" s="10">
+        <v>7402233</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>2012</v>
+      </c>
+      <c r="B8" s="9">
+        <v>43290</v>
+      </c>
+      <c r="C8" s="10">
+        <v>6439072</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>2011</v>
+      </c>
+      <c r="B9" s="9">
+        <v>31271</v>
+      </c>
+      <c r="C9" s="10">
+        <v>4831152</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>2010</v>
+      </c>
+      <c r="B10" s="9">
+        <v>27452</v>
+      </c>
+      <c r="C10" s="10">
+        <v>4174877</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>2009</v>
+      </c>
+      <c r="B11" s="9">
+        <v>27326</v>
+      </c>
+      <c r="C11" s="10">
+        <v>3869594</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>2008</v>
+      </c>
+      <c r="B12" s="9">
+        <v>42728</v>
+      </c>
+      <c r="C12" s="10">
+        <v>5785367</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>2007</v>
+      </c>
+      <c r="B13" s="9">
+        <v>63274</v>
+      </c>
+      <c r="C13" s="10">
+        <v>8291959</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <v>2006</v>
+      </c>
+      <c r="B14" s="9">
+        <v>71719</v>
+      </c>
+      <c r="C14" s="10">
+        <v>9137366</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <v>2005</v>
+      </c>
+      <c r="B15" s="9">
+        <v>62125</v>
+      </c>
+      <c r="C15" s="10">
+        <v>7376807</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
+        <v>2004</v>
+      </c>
+      <c r="B16" s="9">
+        <v>56036</v>
+      </c>
+      <c r="C16" s="10">
+        <v>6499425</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
+        <v>2003</v>
+      </c>
+      <c r="B17" s="9">
+        <v>56571</v>
+      </c>
+      <c r="C17" s="10">
+        <v>5939092</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A18" s="7">
+        <v>2002</v>
+      </c>
+      <c r="B18" s="9">
+        <v>47037</v>
+      </c>
+      <c r="C18" s="10">
+        <v>5146453</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
+        <v>2001</v>
+      </c>
+      <c r="B19" s="9">
+        <v>37569</v>
+      </c>
+      <c r="C19" s="10">
+        <v>4440651</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
+        <v>2000</v>
+      </c>
+      <c r="B20" s="9">
+        <v>35900</v>
+      </c>
+      <c r="C20" s="10">
+        <v>4207090</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD78E4A4-709A-EB40-9646-A5D4E0EB5055}">
   <dimension ref="A2:O43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I43" sqref="I43"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -596,7 +872,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="86" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="C5" t="s">
         <v>1</v>
@@ -613,7 +889,7 @@
       <c r="G5" t="s">
         <v>5</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="6" t="s">
         <v>6</v>
       </c>
       <c r="O5" s="3"/>
@@ -1096,7 +1372,7 @@
         <v>8</v>
       </c>
       <c r="C25" s="1">
-        <v>869594</v>
+        <v>3869594</v>
       </c>
       <c r="D25">
         <v>3566712</v>

</xml_diff>